<commit_message>
Add wham model script, data, and outputs
</commit_message>
<xml_diff>
--- a/Results/WHAM/tables.xlsx
+++ b/Results/WHAM/tables.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62DCC93-3EFC-4F10-8341-7D3A8E488E6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="4275"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new" sheetId="3" r:id="rId1"/>
+    <sheet name="old" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="56">
   <si>
     <t>par</t>
   </si>
@@ -141,15 +143,24 @@
     <t>RW</t>
   </si>
   <si>
+    <t>RW + Cov</t>
+  </si>
+  <si>
     <t>RW sigma</t>
   </si>
   <si>
     <t>--</t>
   </si>
   <si>
+    <t>Cov</t>
+  </si>
+  <si>
     <t>ΔAIC</t>
   </si>
   <si>
+    <t>RW sd</t>
+  </si>
+  <si>
     <t>% variance reduction</t>
   </si>
   <si>
@@ -168,103 +179,28 @@
     <t>fit3...20</t>
   </si>
   <si>
-    <t>RW + Covariate</t>
-  </si>
-  <si>
-    <t>Covariate</t>
-  </si>
-  <si>
-    <t>Constant q</t>
-  </si>
-  <si>
-    <r>
-      <t>Mismatch</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>med</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SP</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>30_wt</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SST</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Mar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RW st. dev. (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>σ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Noise1</t>
-  </si>
-  <si>
-    <t>Noise2</t>
+    <t xml:space="preserve">updated 2023-12-22 </t>
+  </si>
+  <si>
+    <t>using wham version v1.0.6</t>
+  </si>
+  <si>
+    <t>This came from runs on 2023-04-07</t>
+  </si>
+  <si>
+    <t>Unknown version of WHAM, probably based off the 'growth' fork</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,20 +214,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -308,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -365,23 +287,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -396,6 +307,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -405,28 +318,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -707,26 +598,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:U44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6425FD8D-E6DA-4CC7-9660-D1A1A5A064A5}">
+  <dimension ref="B1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -764,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
@@ -772,16 +670,16 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <v>-1.08550996351838</v>
+        <v>-1.0794563484180599</v>
       </c>
       <c r="F6">
-        <v>0.19414648237104401</v>
+        <v>0.19458330004879601</v>
       </c>
       <c r="G6">
-        <v>-1.4660370689656299</v>
+        <v>-1.4608396165137001</v>
       </c>
       <c r="H6">
-        <v>-0.70498285807113104</v>
+        <v>-0.69807308032242499</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -799,14 +697,14 @@
       </c>
       <c r="O6" s="2">
         <f>ROUND(EXP(H6),2)</f>
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="P6" s="1">
         <f>M6^2</f>
         <v>0.11560000000000002</v>
       </c>
     </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
@@ -814,16 +712,16 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <v>-1.4994719636164999</v>
+        <v>-1.48150004140185</v>
       </c>
       <c r="F7">
-        <v>0.26765133162735</v>
+        <v>0.267394231010602</v>
       </c>
       <c r="G7">
-        <v>-2.0240685736061099</v>
+        <v>-2.0055927341826298</v>
       </c>
       <c r="H7">
-        <v>-0.97487535362689604</v>
+        <v>-0.95740734862106602</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
@@ -833,26 +731,26 @@
       </c>
       <c r="M7" s="2">
         <f t="shared" ref="M7:M15" si="0">ROUND(EXP(E7),2)</f>
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="N7" s="2">
-        <f t="shared" ref="N7:N15" si="1">ROUND(EXP(G7),2)</f>
+        <f t="shared" ref="N7:O15" si="1">ROUND(EXP(G7),2)</f>
         <v>0.13</v>
       </c>
       <c r="O7" s="2">
-        <f t="shared" ref="O7:O15" si="2">ROUND(EXP(H7),2)</f>
+        <f t="shared" si="1"/>
         <v>0.38</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ref="P7:P15" si="3">M7^2</f>
-        <v>4.8399999999999999E-2</v>
+        <f t="shared" ref="P7:P15" si="2">M7^2</f>
+        <v>5.2900000000000003E-2</v>
       </c>
       <c r="Q7" s="3">
         <f>(P6-P7)/P6</f>
-        <v>0.5813148788927337</v>
-      </c>
-    </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+        <v>0.54238754325259519</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>3</v>
       </c>
@@ -860,16 +758,16 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>-1.08550987013342</v>
+        <v>-1.0794667298388301</v>
       </c>
       <c r="F8">
-        <v>0.19414772325384</v>
+        <v>0.194588847665326</v>
       </c>
       <c r="G8">
-        <v>-1.46603940771095</v>
+        <v>-1.4608608712628699</v>
       </c>
       <c r="H8">
-        <v>-0.70498033255589299</v>
+        <v>-0.69807258841479203</v>
       </c>
       <c r="I8" t="s">
         <v>8</v>
@@ -886,15 +784,15 @@
         <v>0.23</v>
       </c>
       <c r="O8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="1">
         <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="3"/>
         <v>0.11560000000000002</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>4</v>
       </c>
@@ -902,16 +800,16 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <v>-1.76056114347266</v>
+        <v>-1.75762250583688</v>
       </c>
       <c r="F9">
-        <v>0.28979424739863702</v>
+        <v>0.29446923423819099</v>
       </c>
       <c r="G9">
-        <v>-2.32855786837399</v>
+        <v>-2.3347822049437301</v>
       </c>
       <c r="H9">
-        <v>-1.19256441857133</v>
+        <v>-1.18046280673002</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
@@ -928,19 +826,19 @@
         <v>0.1</v>
       </c>
       <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.31</v>
+      </c>
+      <c r="P9" s="1">
         <f t="shared" si="2"/>
-        <v>0.3</v>
-      </c>
-      <c r="P9" s="1">
-        <f t="shared" si="3"/>
         <v>2.8900000000000006E-2</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" ref="Q9" si="4">(P8-P9)/P8</f>
+        <f t="shared" ref="Q9" si="3">(P8-P9)/P8</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>5</v>
       </c>
@@ -948,41 +846,41 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>-1.0855100565231299</v>
+        <v>-1.07945667069019</v>
       </c>
       <c r="F10">
-        <v>0.19414610933632601</v>
+        <v>0.19458342761956901</v>
       </c>
       <c r="G10">
-        <v>-1.4660364308223299</v>
+        <v>-1.4608401888245499</v>
       </c>
       <c r="H10">
-        <v>-0.70498368222393504</v>
+        <v>-0.69807315255583502</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" ref="M10:M11" si="5">ROUND(EXP(E10),2)</f>
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
       <c r="N10" s="2">
-        <f t="shared" ref="N10:N11" si="6">ROUND(EXP(G10),2)</f>
+        <f t="shared" si="1"/>
         <v>0.23</v>
       </c>
       <c r="O10" s="2">
-        <f t="shared" ref="O10:O11" si="7">ROUND(EXP(H10),2)</f>
-        <v>0.49</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="P10" s="1">
-        <f t="shared" ref="P10:P11" si="8">M10^2</f>
+        <f t="shared" si="2"/>
         <v>0.11560000000000002</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>6</v>
       </c>
@@ -990,45 +888,45 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <v>-1.12772192110806</v>
+        <v>-1.1174740719413701</v>
       </c>
       <c r="F11">
-        <v>0.202632951707167</v>
+        <v>0.20242691110035299</v>
       </c>
       <c r="G11">
-        <v>-1.5248825064541001</v>
+        <v>-1.5142308176980599</v>
       </c>
       <c r="H11">
-        <v>-0.73056133576200999</v>
+        <v>-0.72071732618468098</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="5"/>
-        <v>0.32</v>
+        <f t="shared" si="0"/>
+        <v>0.33</v>
       </c>
       <c r="N11" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>0.22</v>
       </c>
       <c r="O11" s="2">
-        <f t="shared" si="7"/>
-        <v>0.48</v>
+        <f t="shared" si="1"/>
+        <v>0.49</v>
       </c>
       <c r="P11" s="1">
-        <f t="shared" si="8"/>
-        <v>0.1024</v>
+        <f t="shared" si="2"/>
+        <v>0.10890000000000001</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" ref="Q11" si="9">(P10-P11)/P10</f>
-        <v>0.11418685121107279</v>
-      </c>
-    </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+        <f t="shared" ref="Q11" si="4">(P10-P11)/P10</f>
+        <v>5.7958477508650609E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>7</v>
       </c>
@@ -1036,16 +934,16 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <v>-1.0855098673685699</v>
+        <v>-1.07946126991344</v>
       </c>
       <c r="F12">
-        <v>0.19414743639933299</v>
+        <v>0.19458600566176701</v>
       </c>
       <c r="G12">
-        <v>-1.4660388427112601</v>
+        <v>-1.4608498410105</v>
       </c>
       <c r="H12">
-        <v>-0.704980892025874</v>
+        <v>-0.69807269881637501</v>
       </c>
       <c r="I12" t="s">
         <v>8</v>
@@ -1062,15 +960,15 @@
         <v>0.23</v>
       </c>
       <c r="O12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="1">
         <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-      <c r="P12" s="1">
-        <f t="shared" si="3"/>
         <v>0.11560000000000002</v>
       </c>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>8</v>
       </c>
@@ -1078,16 +976,16 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>-1.08484396094806</v>
+        <v>-1.08293950231021</v>
       </c>
       <c r="F13">
-        <v>0.193918818016103</v>
+        <v>0.19412134754463001</v>
       </c>
       <c r="G13">
-        <v>-1.4649248442596201</v>
+        <v>-1.46341734349769</v>
       </c>
       <c r="H13">
-        <v>-0.70476307763649504</v>
+        <v>-0.70246166112274</v>
       </c>
       <c r="I13" t="s">
         <v>10</v>
@@ -1104,19 +1002,19 @@
         <v>0.23</v>
       </c>
       <c r="O13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P13" s="1">
         <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-      <c r="P13" s="1">
-        <f t="shared" si="3"/>
         <v>0.11560000000000002</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13" si="10">(P12-P13)/P12</f>
+        <f t="shared" ref="Q13" si="5">(P12-P13)/P12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>9</v>
       </c>
@@ -1124,16 +1022,16 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <v>-1.0855099185310599</v>
+        <v>-1.07946290468933</v>
       </c>
       <c r="F14">
-        <v>0.19414676763817601</v>
+        <v>0.194586868163479</v>
       </c>
       <c r="G14">
-        <v>-1.4660375831018799</v>
+        <v>-1.4608531662897499</v>
       </c>
       <c r="H14">
-        <v>-0.70498225396023195</v>
+        <v>-0.69807264308890704</v>
       </c>
       <c r="I14" t="s">
         <v>8</v>
@@ -1150,15 +1048,15 @@
         <v>0.23</v>
       </c>
       <c r="O14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="P14" s="1">
         <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-      <c r="P14" s="1">
-        <f t="shared" si="3"/>
         <v>0.11560000000000002</v>
       </c>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>10</v>
       </c>
@@ -1166,16 +1064,16 @@
         <v>7</v>
       </c>
       <c r="E15">
-        <v>-1.10557669353528</v>
+        <v>-1.1002730071161599</v>
       </c>
       <c r="F15">
-        <v>0.198425935797441</v>
+        <v>0.19886029801271199</v>
       </c>
       <c r="G15">
-        <v>-1.49449152769826</v>
+        <v>-1.49003919122107</v>
       </c>
       <c r="H15">
-        <v>-0.71666185937229099</v>
+        <v>-0.71050682301124102</v>
       </c>
       <c r="I15" t="s">
         <v>10</v>
@@ -1189,18 +1087,18 @@
       </c>
       <c r="N15" s="2">
         <f t="shared" si="1"/>
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="O15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.49</v>
+      </c>
+      <c r="P15" s="1">
         <f t="shared" si="2"/>
-        <v>0.49</v>
-      </c>
-      <c r="P15" s="1">
-        <f t="shared" si="3"/>
         <v>0.10890000000000001</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" ref="Q15" si="11">(P14-P15)/P14</f>
+        <f t="shared" ref="Q15" si="6">(P14-P15)/P14</f>
         <v>5.7958477508650609E-2</v>
       </c>
     </row>
@@ -1222,16 +1120,24 @@
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K21" s="8"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N21" s="21"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
+      <c r="M21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="S21" s="8"/>
       <c r="T21" s="4" t="s">
         <v>9</v>
@@ -1240,7 +1146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="4:21" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>5</v>
       </c>
@@ -1255,30 +1161,30 @@
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="N22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="O22" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="P22" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="R22" s="19" t="s">
-        <v>54</v>
+      <c r="M22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="S22" s="8"/>
       <c r="T22" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="U22" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.25">
@@ -1292,44 +1198,47 @@
         <v>9</v>
       </c>
       <c r="G23">
-        <v>116.4</v>
+        <v>114.5</v>
       </c>
       <c r="H23">
-        <v>2023.9</v>
+        <v>2021.1</v>
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="M23" s="5">
-        <f>G23</f>
-        <v>116.4</v>
+        <f>G24</f>
+        <v>8.3000000000000007</v>
       </c>
       <c r="N23" s="5">
-        <f>G27</f>
-        <v>120.5</v>
+        <f>G28</f>
+        <v>12.3</v>
       </c>
       <c r="O23" s="5">
-        <f>G31</f>
-        <v>107.8</v>
-      </c>
-      <c r="P23" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q23" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="R23" s="18" t="s">
-        <v>41</v>
+        <f>G32</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="14">
+        <f>M6</f>
+        <v>0.34</v>
+      </c>
+      <c r="Q23" s="10">
+        <f>M8</f>
+        <v>0.34</v>
+      </c>
+      <c r="R23" s="10">
+        <f>M10</f>
+        <v>0.34</v>
       </c>
       <c r="S23" s="8"/>
       <c r="T23" s="5" t="str">
         <f>CONCATENATE(M6," (",N6,"-",O6,")")</f>
-        <v>0.34 (0.23-0.49)</v>
+        <v>0.34 (0.23-0.5)</v>
       </c>
       <c r="U23" s="5" t="str">
         <f>CONCATENATE(M8," (",N8,"-",O8,")")</f>
-        <v>0.34 (0.23-0.49)</v>
+        <v>0.34 (0.23-0.5)</v>
       </c>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.25">
@@ -1343,45 +1252,42 @@
         <v>9</v>
       </c>
       <c r="G24">
-        <v>8.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H24">
-        <v>1916.1</v>
+        <v>1914.9</v>
       </c>
       <c r="K24" s="8"/>
       <c r="L24" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M24" s="5">
-        <f>G24</f>
-        <v>8.6</v>
+        <f>G25</f>
+        <v>13.8</v>
       </c>
       <c r="N24" s="5">
-        <f>G28</f>
-        <v>12.7</v>
+        <f>G29</f>
+        <v>6.4</v>
       </c>
       <c r="O24" s="5">
-        <f>G32</f>
-        <v>0</v>
-      </c>
-      <c r="P24" s="12">
-        <f>M6</f>
-        <v>0.34</v>
-      </c>
-      <c r="Q24" s="10">
-        <f>M8</f>
-        <v>0.34</v>
-      </c>
-      <c r="R24" s="10">
-        <f>M10</f>
-        <v>0.34</v>
+        <f t="shared" ref="O24:O25" si="7">G33</f>
+        <v>71</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="S24" s="8"/>
       <c r="T24" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="4:21" x14ac:dyDescent="0.25">
@@ -1398,41 +1304,44 @@
         <v>13.8</v>
       </c>
       <c r="H25">
-        <v>1921.3</v>
+        <v>1920.4</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="5">
-        <f>G25</f>
-        <v>13.8</v>
-      </c>
-      <c r="N25" s="5">
-        <f>G29</f>
-        <v>7.1</v>
-      </c>
-      <c r="O25" s="5">
-        <f t="shared" ref="O25:O26" si="12">G33</f>
-        <v>71.7</v>
-      </c>
-      <c r="P25" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q25" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>41</v>
+      <c r="L25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="7">
+        <f>G26</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="7">
+        <f>G30</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="16">
+        <f>M7</f>
+        <v>0.23</v>
+      </c>
+      <c r="Q25" s="9">
+        <f>M9</f>
+        <v>0.17</v>
+      </c>
+      <c r="R25" s="9">
+        <f>M11</f>
+        <v>0.33</v>
       </c>
       <c r="S25" s="8"/>
       <c r="T25" s="6" t="str">
         <f>CONCATENATE(M7," (",N7,"-",O7,")")</f>
-        <v>0.22 (0.13-0.38)</v>
+        <v>0.23 (0.13-0.38)</v>
       </c>
       <c r="U25" s="6" t="str">
         <f>CONCATENATE(M9," (",N9,"-",O9,")")</f>
-        <v>0.17 (0.1-0.3)</v>
+        <v>0.17 (0.1-0.31)</v>
       </c>
     </row>
     <row r="26" spans="4:21" x14ac:dyDescent="0.25">
@@ -1449,35 +1358,26 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>1907.5</v>
+        <v>1906.6</v>
       </c>
       <c r="K26" s="8"/>
-      <c r="L26" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M26" s="7">
-        <f>G26</f>
-        <v>0</v>
-      </c>
-      <c r="N26" s="7">
-        <f>G30</f>
-        <v>0</v>
-      </c>
-      <c r="O26" s="7">
-        <f t="shared" si="12"/>
-        <v>0.9</v>
-      </c>
-      <c r="P26" s="14">
-        <f>M7</f>
-        <v>0.22</v>
-      </c>
-      <c r="Q26" s="9">
-        <f>M9</f>
-        <v>0.17</v>
-      </c>
-      <c r="R26" s="9">
-        <f>M11</f>
-        <v>0.32</v>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P26" s="18">
+        <f>Q7</f>
+        <v>0.54238754325259519</v>
+      </c>
+      <c r="Q26" s="18">
+        <f>Q9</f>
+        <v>0.75</v>
+      </c>
+      <c r="R26" s="18">
+        <f>Q11</f>
+        <v>5.7958477508650609E-2</v>
       </c>
       <c r="S26" s="8"/>
     </row>
@@ -1492,30 +1392,19 @@
         <v>11</v>
       </c>
       <c r="G27">
-        <v>120.5</v>
+        <v>118.5</v>
       </c>
       <c r="H27">
-        <v>2005.3</v>
+        <v>2002.5</v>
       </c>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="P27" s="16">
-        <f>Q7</f>
-        <v>0.5813148788927337</v>
-      </c>
-      <c r="Q27" s="16">
-        <f>Q9</f>
-        <v>0.75</v>
-      </c>
-      <c r="R27" s="16">
-        <f>Q11</f>
-        <v>0.11418685121107279</v>
-      </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -1528,10 +1417,10 @@
         <v>11</v>
       </c>
       <c r="G28">
-        <v>12.7</v>
+        <v>12.3</v>
       </c>
       <c r="H28">
-        <v>1897.5</v>
+        <v>1896.3</v>
       </c>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -1553,15 +1442,11 @@
         <v>11</v>
       </c>
       <c r="G29">
-        <v>7.1</v>
+        <v>6.4</v>
       </c>
       <c r="H29">
-        <v>1891.9</v>
-      </c>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
+        <v>1890.4</v>
+      </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -1580,11 +1465,8 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>1884.8</v>
-      </c>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
+        <v>1884</v>
+      </c>
     </row>
     <row r="31" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
@@ -1594,13 +1476,13 @@
         <v>22</v>
       </c>
       <c r="F31" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G31">
-        <v>107.8</v>
+        <v>106.2</v>
       </c>
       <c r="H31">
-        <v>2036.3</v>
+        <v>2033.6</v>
       </c>
     </row>
     <row r="32" spans="4:21" x14ac:dyDescent="0.25">
@@ -1611,16 +1493,28 @@
         <v>8</v>
       </c>
       <c r="F32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G32">
         <v>0</v>
       </c>
       <c r="H32">
-        <v>1928.5</v>
-      </c>
-    </row>
-    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+        <v>1927.4</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>33</v>
       </c>
@@ -1628,7 +1522,1099 @@
         <v>25</v>
       </c>
       <c r="F33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33">
+        <v>71</v>
+      </c>
+      <c r="H33">
+        <v>1998.4</v>
+      </c>
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1928.4</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>106.2</v>
+      </c>
+      <c r="H35">
+        <v>2007.5</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>1901.3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37">
+        <v>102</v>
+      </c>
+      <c r="H37">
+        <v>2003.3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>1903.3</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>106.2</v>
+      </c>
+      <c r="H39">
+        <v>2038.3</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>1932.1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F41" t="s">
+        <v>13</v>
+      </c>
+      <c r="G41">
+        <v>102.8</v>
+      </c>
+      <c r="H41">
+        <v>2034.9</v>
+      </c>
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>51</v>
+      </c>
+      <c r="E42" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42">
+        <v>1.5</v>
+      </c>
+      <c r="H42">
+        <v>1933.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:U42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>-1.08550996351838</v>
+      </c>
+      <c r="F6">
+        <v>0.19414648237104401</v>
+      </c>
+      <c r="G6">
+        <v>-1.4660370689656299</v>
+      </c>
+      <c r="H6">
+        <v>-0.70498285807113104</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="2">
+        <f>ROUND(EXP(E6),2)</f>
+        <v>0.34</v>
+      </c>
+      <c r="N6" s="2">
+        <f>ROUND(EXP(G6),2)</f>
+        <v>0.23</v>
+      </c>
+      <c r="O6" s="2">
+        <f>ROUND(EXP(H6),2)</f>
+        <v>0.49</v>
+      </c>
+      <c r="P6" s="1">
+        <f>M6^2</f>
+        <v>0.11560000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7">
+        <v>-1.4994719636164999</v>
+      </c>
+      <c r="F7">
+        <v>0.26765133162735</v>
+      </c>
+      <c r="G7">
+        <v>-2.0240685736061099</v>
+      </c>
+      <c r="H7">
+        <v>-0.97487535362689604</v>
+      </c>
+      <c r="I7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M15" si="0">ROUND(EXP(E7),2)</f>
+        <v>0.22</v>
+      </c>
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N15" si="1">ROUND(EXP(G7),2)</f>
+        <v>0.13</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" ref="O7:O15" si="2">ROUND(EXP(H7),2)</f>
+        <v>0.38</v>
+      </c>
+      <c r="P7" s="1">
+        <f t="shared" ref="P7:P15" si="3">M7^2</f>
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>(P6-P7)/P6</f>
+        <v>0.5813148788927337</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>-1.08550987013342</v>
+      </c>
+      <c r="F8">
+        <v>0.19414772325384</v>
+      </c>
+      <c r="G8">
+        <v>-1.46603940771095</v>
+      </c>
+      <c r="H8">
+        <v>-0.70498033255589299</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="P8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11560000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>-1.76056114347266</v>
+      </c>
+      <c r="F9">
+        <v>0.28979424739863702</v>
+      </c>
+      <c r="G9">
+        <v>-2.32855786837399</v>
+      </c>
+      <c r="H9">
+        <v>-1.19256441857133</v>
+      </c>
+      <c r="I9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="P9" s="1">
+        <f t="shared" si="3"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" ref="Q9" si="4">(P8-P9)/P8</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>-1.0855100565231299</v>
+      </c>
+      <c r="F10">
+        <v>0.19414610933632601</v>
+      </c>
+      <c r="G10">
+        <v>-1.4660364308223299</v>
+      </c>
+      <c r="H10">
+        <v>-0.70498368222393504</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" ref="M10:M11" si="5">ROUND(EXP(E10),2)</f>
+        <v>0.34</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" ref="N10:N11" si="6">ROUND(EXP(G10),2)</f>
+        <v>0.23</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" ref="O10:O11" si="7">ROUND(EXP(H10),2)</f>
+        <v>0.49</v>
+      </c>
+      <c r="P10" s="1">
+        <f t="shared" ref="P10:P11" si="8">M10^2</f>
+        <v>0.11560000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>-1.12772192110806</v>
+      </c>
+      <c r="F11">
+        <v>0.202632951707167</v>
+      </c>
+      <c r="G11">
+        <v>-1.5248825064541001</v>
+      </c>
+      <c r="H11">
+        <v>-0.73056133576200999</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="5"/>
+        <v>0.32</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="6"/>
+        <v>0.22</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="7"/>
+        <v>0.48</v>
+      </c>
+      <c r="P11" s="1">
+        <f t="shared" si="8"/>
+        <v>0.1024</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" ref="Q11" si="9">(P10-P11)/P10</f>
+        <v>0.11418685121107279</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>-1.0855098673685699</v>
+      </c>
+      <c r="F12">
+        <v>0.19414743639933299</v>
+      </c>
+      <c r="G12">
+        <v>-1.4660388427112601</v>
+      </c>
+      <c r="H12">
+        <v>-0.704980892025874</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="P12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11560000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>-1.08484396094806</v>
+      </c>
+      <c r="F13">
+        <v>0.193918818016103</v>
+      </c>
+      <c r="G13">
+        <v>-1.4649248442596201</v>
+      </c>
+      <c r="H13">
+        <v>-0.70476307763649504</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="P13" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11560000000000002</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" ref="Q13" si="10">(P12-P13)/P12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>-1.0855099185310599</v>
+      </c>
+      <c r="F14">
+        <v>0.19414676763817601</v>
+      </c>
+      <c r="G14">
+        <v>-1.4660375831018799</v>
+      </c>
+      <c r="H14">
+        <v>-0.70498225396023195</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.34</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.23</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="P14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.11560000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>-1.10557669353528</v>
+      </c>
+      <c r="F15">
+        <v>0.198425935797441</v>
+      </c>
+      <c r="G15">
+        <v>-1.49449152769826</v>
+      </c>
+      <c r="H15">
+        <v>-0.71666185937229099</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="2"/>
+        <v>0.49</v>
+      </c>
+      <c r="P15" s="1">
+        <f t="shared" si="3"/>
+        <v>0.10890000000000001</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" ref="Q15" si="11">(P14-P15)/P14</f>
+        <v>5.7958477508650609E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="K21" s="8"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4" t="s">
         <v>44</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="T21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="8"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S22" s="8"/>
+      <c r="T22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23">
+        <v>116.4</v>
+      </c>
+      <c r="H23">
+        <v>2023.9</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="5">
+        <f>G24</f>
+        <v>8.6</v>
+      </c>
+      <c r="N23" s="5">
+        <f>G28</f>
+        <v>12.7</v>
+      </c>
+      <c r="O23" s="5">
+        <f>G32</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="14">
+        <f>M6</f>
+        <v>0.34</v>
+      </c>
+      <c r="Q23" s="10">
+        <f>M8</f>
+        <v>0.34</v>
+      </c>
+      <c r="R23" s="10">
+        <f>M10</f>
+        <v>0.34</v>
+      </c>
+      <c r="S23" s="8"/>
+      <c r="T23" s="5" t="str">
+        <f>CONCATENATE(M6," (",N6,"-",O6,")")</f>
+        <v>0.34 (0.23-0.49)</v>
+      </c>
+      <c r="U23" s="5" t="str">
+        <f>CONCATENATE(M8," (",N8,"-",O8,")")</f>
+        <v>0.34 (0.23-0.49)</v>
+      </c>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>8.6</v>
+      </c>
+      <c r="H24">
+        <v>1916.1</v>
+      </c>
+      <c r="K24" s="8"/>
+      <c r="L24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M24" s="5">
+        <f>G25</f>
+        <v>13.8</v>
+      </c>
+      <c r="N24" s="5">
+        <f>G29</f>
+        <v>7.1</v>
+      </c>
+      <c r="O24" s="5">
+        <f t="shared" ref="O24:O25" si="12">G33</f>
+        <v>71.7</v>
+      </c>
+      <c r="P24" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="S24" s="8"/>
+      <c r="T24" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>13.8</v>
+      </c>
+      <c r="H25">
+        <v>1921.3</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="7">
+        <f>G26</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="7">
+        <f>G30</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" si="12"/>
+        <v>0.9</v>
+      </c>
+      <c r="P25" s="16">
+        <f>M7</f>
+        <v>0.22</v>
+      </c>
+      <c r="Q25" s="9">
+        <f>M9</f>
+        <v>0.17</v>
+      </c>
+      <c r="R25" s="9">
+        <f>M11</f>
+        <v>0.32</v>
+      </c>
+      <c r="S25" s="8"/>
+      <c r="T25" s="6" t="str">
+        <f>CONCATENATE(M7," (",N7,"-",O7,")")</f>
+        <v>0.22 (0.13-0.38)</v>
+      </c>
+      <c r="U25" s="6" t="str">
+        <f>CONCATENATE(M9," (",N9,"-",O9,")")</f>
+        <v>0.17 (0.1-0.3)</v>
+      </c>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1907.5</v>
+      </c>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P26" s="18">
+        <f>Q7</f>
+        <v>0.5813148788927337</v>
+      </c>
+      <c r="Q26" s="18">
+        <f>Q9</f>
+        <v>0.75</v>
+      </c>
+      <c r="R26" s="18">
+        <f>Q11</f>
+        <v>0.11418685121107279</v>
+      </c>
+      <c r="S26" s="8"/>
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27">
+        <v>120.5</v>
+      </c>
+      <c r="H27">
+        <v>2005.3</v>
+      </c>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28">
+        <v>12.7</v>
+      </c>
+      <c r="H28">
+        <v>1897.5</v>
+      </c>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29">
+        <v>7.1</v>
+      </c>
+      <c r="H29">
+        <v>1891.9</v>
+      </c>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1884.8</v>
+      </c>
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G31">
+        <v>107.8</v>
+      </c>
+      <c r="H31">
+        <v>2036.3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>47</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1928.5</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
       </c>
       <c r="G33">
         <v>71.7</v>
@@ -1636,12 +2622,8 @@
       <c r="H33">
         <v>2000.2</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>34</v>
       </c>
@@ -1649,7 +2631,7 @@
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G34">
         <v>0.9</v>
@@ -1658,7 +2640,7 @@
         <v>1929.4</v>
       </c>
     </row>
-    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>35</v>
       </c>
@@ -1675,7 +2657,7 @@
         <v>2010.2</v>
       </c>
     </row>
-    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>36</v>
       </c>
@@ -1691,16 +2673,8 @@
       <c r="H36">
         <v>1902.5</v>
       </c>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-    </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>37</v>
       </c>
@@ -1716,19 +2690,8 @@
       <c r="H37">
         <v>2006</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N37" s="22"/>
-      <c r="O37" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="8"/>
-    </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>38</v>
       </c>
@@ -1744,25 +2707,10 @@
       <c r="H38">
         <v>1904.4</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="N38" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="O38" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="P38" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q38" s="8"/>
-    </row>
-    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
         <v>22</v>
@@ -1776,29 +2724,10 @@
       <c r="H39">
         <v>2041.1</v>
       </c>
-      <c r="K39" s="8"/>
-      <c r="L39" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="M39" s="5">
-        <f>G35</f>
-        <v>107.7</v>
-      </c>
-      <c r="N39" s="5">
-        <f>G39</f>
-        <v>107.8</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="P39" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q39" s="8"/>
-    </row>
-    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1812,31 +2741,10 @@
       <c r="H40">
         <v>1933.3</v>
       </c>
-      <c r="K40" s="8"/>
-      <c r="L40" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M40" s="5">
-        <f>G36</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="5">
-        <f>G40</f>
-        <v>0</v>
-      </c>
-      <c r="O40" s="12">
-        <f>M12</f>
-        <v>0.34</v>
-      </c>
-      <c r="P40" s="10">
-        <f>M14</f>
-        <v>0.34</v>
-      </c>
-      <c r="Q40" s="8"/>
-    </row>
-    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
         <v>25</v>
@@ -1850,29 +2758,10 @@
       <c r="H41">
         <v>2037.7</v>
       </c>
-      <c r="K41" s="8"/>
-      <c r="L41" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M41" s="5">
-        <f>G37</f>
-        <v>103.5</v>
-      </c>
-      <c r="N41" s="5">
-        <f>G41</f>
-        <v>104.4</v>
-      </c>
-      <c r="O41" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="P41" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q41" s="8"/>
-    </row>
-    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
         <v>10</v>
@@ -1886,64 +2775,8 @@
       <c r="H42">
         <v>1934.8</v>
       </c>
-      <c r="K42" s="8"/>
-      <c r="L42" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="M42" s="7">
-        <f>G38</f>
-        <v>1.9</v>
-      </c>
-      <c r="N42" s="7">
-        <f>G42</f>
-        <v>1.5</v>
-      </c>
-      <c r="O42" s="14">
-        <f>M13</f>
-        <v>0.34</v>
-      </c>
-      <c r="P42" s="9">
-        <f>M15</f>
-        <v>0.33</v>
-      </c>
-      <c r="Q42" s="8"/>
-    </row>
-    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O43" s="24">
-        <f>Q13</f>
-        <v>0</v>
-      </c>
-      <c r="P43" s="16">
-        <f>Q15</f>
-        <v>5.7958477508650609E-2</v>
-      </c>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
-    </row>
-    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="K44" s="8"/>
-      <c r="L44" s="8"/>
-      <c r="M44" s="8"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="M37:N37"/>
-    <mergeCell ref="O37:P37"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update figures and table with final WHAM run
</commit_message>
<xml_diff>
--- a/Results/WHAM/tables.xlsx
+++ b/Results/WHAM/tables.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20402"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62DCC93-3EFC-4F10-8341-7D3A8E488E6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="3" r:id="rId1"/>
     <sheet name="old" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="65">
   <si>
     <t>par</t>
   </si>
@@ -189,18 +188,105 @@
   </si>
   <si>
     <t>Unknown version of WHAM, probably based off the 'growth' fork</t>
+  </si>
+  <si>
+    <r>
+      <t>RW st. dev. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>σ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Noise1</t>
+  </si>
+  <si>
+    <t>Noise2</t>
+  </si>
+  <si>
+    <t>Constant q</t>
+  </si>
+  <si>
+    <t>Covariate</t>
+  </si>
+  <si>
+    <t>RW + Covariate</t>
+  </si>
+  <si>
+    <r>
+      <t>SP</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30_wt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mismatch</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>med</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SST</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mar</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +295,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -230,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -287,12 +387,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -318,6 +429,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,19 +732,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6425FD8D-E6DA-4CC7-9660-D1A1A5A064A5}">
-  <dimension ref="B1:U42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:U43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K36" sqref="K36:Q43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" customWidth="1"/>
     <col min="16" max="16" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1120,24 +1254,16 @@
     <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="K21" s="8"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="4" t="s">
+      <c r="M21" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="N21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="P21" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="N21" s="19"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
       <c r="S21" s="8"/>
       <c r="T21" s="4" t="s">
         <v>9</v>
@@ -1146,7 +1272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:21" ht="18" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
         <v>5</v>
       </c>
@@ -1161,23 +1287,23 @@
       </c>
       <c r="K22" s="8"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="R22" s="6" t="s">
-        <v>47</v>
+      <c r="M22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="O22" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="P22" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q22" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="R22" s="22" t="s">
+        <v>64</v>
       </c>
       <c r="S22" s="8"/>
       <c r="T22" s="6" t="s">
@@ -1205,31 +1331,28 @@
       </c>
       <c r="K23" s="8"/>
       <c r="L23" s="5" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="M23" s="5">
-        <f>G24</f>
-        <v>8.3000000000000007</v>
+        <f>G23</f>
+        <v>114.5</v>
       </c>
       <c r="N23" s="5">
-        <f>G28</f>
-        <v>12.3</v>
+        <f>G27</f>
+        <v>118.5</v>
       </c>
       <c r="O23" s="5">
-        <f>G32</f>
-        <v>0</v>
-      </c>
-      <c r="P23" s="14">
-        <f>M6</f>
-        <v>0.34</v>
-      </c>
-      <c r="Q23" s="10">
-        <f>M8</f>
-        <v>0.34</v>
-      </c>
-      <c r="R23" s="10">
-        <f>M10</f>
-        <v>0.34</v>
+        <f>G31</f>
+        <v>106.2</v>
+      </c>
+      <c r="P23" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q23" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R23" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="S23" s="8"/>
       <c r="T23" s="5" t="str">
@@ -1259,28 +1382,31 @@
       </c>
       <c r="K24" s="8"/>
       <c r="L24" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M24" s="5">
-        <f>G25</f>
-        <v>13.8</v>
+        <f>G24</f>
+        <v>8.3000000000000007</v>
       </c>
       <c r="N24" s="5">
-        <f>G29</f>
-        <v>6.4</v>
+        <f>G28</f>
+        <v>12.3</v>
       </c>
       <c r="O24" s="5">
-        <f t="shared" ref="O24:O25" si="7">G33</f>
-        <v>71</v>
-      </c>
-      <c r="P24" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="R24" s="11" t="s">
-        <v>42</v>
+        <f>G32</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="14">
+        <f>M6</f>
+        <v>0.34</v>
+      </c>
+      <c r="Q24" s="10">
+        <f>M8</f>
+        <v>0.34</v>
+      </c>
+      <c r="R24" s="10">
+        <f>M10</f>
+        <v>0.34</v>
       </c>
       <c r="S24" s="8"/>
       <c r="T24" s="5" t="s">
@@ -1307,32 +1433,29 @@
         <v>1920.4</v>
       </c>
       <c r="K25" s="8"/>
-      <c r="L25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M25" s="7">
-        <f>G26</f>
-        <v>0</v>
-      </c>
-      <c r="N25" s="7">
-        <f>G30</f>
-        <v>0</v>
-      </c>
-      <c r="O25" s="7">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="P25" s="16">
-        <f>M7</f>
-        <v>0.23</v>
-      </c>
-      <c r="Q25" s="9">
-        <f>M9</f>
-        <v>0.17</v>
-      </c>
-      <c r="R25" s="9">
-        <f>M11</f>
-        <v>0.33</v>
+      <c r="L25" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M25" s="5">
+        <f>G25</f>
+        <v>13.8</v>
+      </c>
+      <c r="N25" s="5">
+        <f>G29</f>
+        <v>6.4</v>
+      </c>
+      <c r="O25" s="5">
+        <f t="shared" ref="O25:O26" si="7">G33</f>
+        <v>71</v>
+      </c>
+      <c r="P25" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q25" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R25" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="S25" s="8"/>
       <c r="T25" s="6" t="str">
@@ -1361,23 +1484,32 @@
         <v>1906.6</v>
       </c>
       <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="P26" s="18">
-        <f>Q7</f>
-        <v>0.54238754325259519</v>
-      </c>
-      <c r="Q26" s="18">
-        <f>Q9</f>
-        <v>0.75</v>
-      </c>
-      <c r="R26" s="18">
-        <f>Q11</f>
-        <v>5.7958477508650609E-2</v>
+      <c r="L26" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M26" s="7">
+        <f>G26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="7">
+        <f>G30</f>
+        <v>0</v>
+      </c>
+      <c r="O26" s="7">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P26" s="16">
+        <f>M7</f>
+        <v>0.23</v>
+      </c>
+      <c r="Q26" s="9">
+        <f>M9</f>
+        <v>0.17</v>
+      </c>
+      <c r="R26" s="9">
+        <f>M11</f>
+        <v>0.33</v>
       </c>
       <c r="S26" s="8"/>
     </row>
@@ -1401,10 +1533,21 @@
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
+      <c r="O27" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="P27" s="18">
+        <f>Q7</f>
+        <v>0.54238754325259519</v>
+      </c>
+      <c r="Q27" s="18">
+        <f>Q9</f>
+        <v>0.75</v>
+      </c>
+      <c r="R27" s="18">
+        <f>Q11</f>
+        <v>5.7958477508650609E-2</v>
+      </c>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
@@ -1447,6 +1590,10 @@
       <c r="H29">
         <v>1890.4</v>
       </c>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
@@ -1514,7 +1661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>33</v>
       </c>
@@ -1524,14 +1671,14 @@
       <c r="F33" t="s">
         <v>47</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="27">
         <v>71</v>
       </c>
       <c r="H33">
         <v>1998.4</v>
       </c>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>34</v>
       </c>
@@ -1548,7 +1695,7 @@
         <v>1928.4</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>35</v>
       </c>
@@ -1565,7 +1712,7 @@
         <v>2007.5</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>36</v>
       </c>
@@ -1581,8 +1728,15 @@
       <c r="H36">
         <v>1901.3</v>
       </c>
-    </row>
-    <row r="37" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="8"/>
+    </row>
+    <row r="37" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>37</v>
       </c>
@@ -1598,8 +1752,19 @@
       <c r="H37">
         <v>2003.3</v>
       </c>
-    </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K37" s="8"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="N37" s="20"/>
+      <c r="O37" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="8"/>
+    </row>
+    <row r="38" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>38</v>
       </c>
@@ -1615,8 +1780,23 @@
       <c r="H38">
         <v>1903.3</v>
       </c>
-    </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K38" s="8"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="N38" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="O38" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="P38" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q38" s="8"/>
+    </row>
+    <row r="39" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>48</v>
       </c>
@@ -1632,8 +1812,27 @@
       <c r="H39">
         <v>2038.3</v>
       </c>
-    </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K39" s="8"/>
+      <c r="L39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="M39" s="5">
+        <f>G35</f>
+        <v>106.2</v>
+      </c>
+      <c r="N39" s="5">
+        <f>G39</f>
+        <v>106.2</v>
+      </c>
+      <c r="O39" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="P39" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q39" s="8"/>
+    </row>
+    <row r="40" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>49</v>
       </c>
@@ -1649,8 +1848,29 @@
       <c r="H40">
         <v>1932.1</v>
       </c>
-    </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K40" s="8"/>
+      <c r="L40" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M40" s="5">
+        <f>G36</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="5">
+        <f>G40</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="14">
+        <f>M12</f>
+        <v>0.34</v>
+      </c>
+      <c r="P40" s="10">
+        <f>M14</f>
+        <v>0.34</v>
+      </c>
+      <c r="Q40" s="8"/>
+    </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>50</v>
       </c>
@@ -1666,8 +1886,27 @@
       <c r="H41">
         <v>2034.9</v>
       </c>
-    </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="K41" s="8"/>
+      <c r="L41" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M41" s="5">
+        <f>G37</f>
+        <v>102</v>
+      </c>
+      <c r="N41" s="5">
+        <f>G41</f>
+        <v>102.8</v>
+      </c>
+      <c r="O41" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="P41" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q41" s="8"/>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>51</v>
       </c>
@@ -1683,17 +1922,61 @@
       <c r="H42">
         <v>1933.6</v>
       </c>
+      <c r="K42" s="8"/>
+      <c r="L42" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M42" s="7">
+        <f>G38</f>
+        <v>2</v>
+      </c>
+      <c r="N42" s="7">
+        <f>G42</f>
+        <v>1.5</v>
+      </c>
+      <c r="O42" s="16">
+        <f>M13</f>
+        <v>0.34</v>
+      </c>
+      <c r="P42" s="9">
+        <f>M15</f>
+        <v>0.33</v>
+      </c>
+      <c r="Q42" s="8"/>
+    </row>
+    <row r="43" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="O43" s="26">
+        <f>Q13</f>
+        <v>0</v>
+      </c>
+      <c r="P43" s="18">
+        <f>Q15</f>
+        <v>5.7958477508650609E-2</v>
+      </c>
+      <c r="Q43" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>